<commit_message>
7,05 data upload przekształcony help i info coś w końcu jest i inne
</commit_message>
<xml_diff>
--- a/datasets/rna-seq szblon.xlsx
+++ b/datasets/rna-seq szblon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\projekt_mgr\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AF342F-8036-4CD3-B531-936977A59903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D824F6C-75AC-4B5C-8E71-B67AACEB5915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="960" windowWidth="12420" windowHeight="13890" tabRatio="818" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" tabRatio="818" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rna-seq szablon" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884A4CF5-F5CA-403B-94EE-B584E0CD0D85}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>